<commit_message>
Lots of shuffling and changes.
</commit_message>
<xml_diff>
--- a/test/grafter/test.xlsx
+++ b/test/grafter/test.xlsx
@@ -34,10 +34,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,13 +76,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,35 +423,36 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2">
         <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
basic polymorphic revisions to open-dataset(s)
</commit_message>
<xml_diff>
--- a/test/grafter/test.xlsx
+++ b/test/grafter/test.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>one</t>
   </si>
@@ -28,6 +29,15 @@
   </si>
   <si>
     <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>six</t>
   </si>
 </sst>
 </file>
@@ -422,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -459,4 +469,46 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>